<commit_message>
A bunch of new metal interference data
</commit_message>
<xml_diff>
--- a/output_file/May Y=0/example.xlsx
+++ b/output_file/May Y=0/example.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
   <si>
     <t>MetalShape</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Control</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -508,16 +511,16 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>5.7947074917335716E-7</v>
+        <v>1.5011101014405675E-6</v>
       </c>
       <c r="D9">
-        <v>3.3658878039038144E-6</v>
+        <v>1.197085756861482E-5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -525,13 +528,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>4.6051638832493007E-7</v>
+        <v>5.7947074917335716E-7</v>
       </c>
       <c r="D10">
-        <v>5.3854028433374753E-6</v>
+        <v>3.3658878039038144E-6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -539,13 +542,13 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>1.4205038478010832E-6</v>
+        <v>4.6051638832493007E-7</v>
       </c>
       <c r="D11">
-        <v>7.6430713903476887E-6</v>
+        <v>5.3854028433374753E-6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -553,13 +556,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>3.2421171726750339E-6</v>
+        <v>1.4205038478010832E-6</v>
       </c>
       <c r="D12">
-        <v>1.5780326137289526E-5</v>
+        <v>7.6430713903476887E-6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -567,13 +570,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>5.2880230770178713E-6</v>
+        <v>3.2421171726750339E-6</v>
       </c>
       <c r="D13">
-        <v>9.6326158829035823E-6</v>
+        <v>1.5780326137289526E-5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -581,13 +584,13 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>2.8061680933257652E-6</v>
+        <v>5.2880230770178713E-6</v>
       </c>
       <c r="D14">
-        <v>3.6577892924771489E-5</v>
+        <v>9.6326158829035823E-6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -595,13 +598,13 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15">
-        <v>1.8797195762635652E-6</v>
+        <v>2.8061680933257652E-6</v>
       </c>
       <c r="D15">
-        <v>1.1754396426082914E-5</v>
+        <v>3.6577892924771489E-5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -609,13 +612,13 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16">
-        <v>1.9335520129461728E-5</v>
+        <v>1.8797195762635652E-6</v>
       </c>
       <c r="D16">
-        <v>4.003789050525927E-3</v>
+        <v>1.1754396426082914E-5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -623,13 +626,13 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C17">
-        <v>2.6254402111760776E-6</v>
+        <v>1.5011101014405675E-6</v>
       </c>
       <c r="D17">
-        <v>1.3703059119475065E-5</v>
+        <v>1.197085756861482E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>